<commit_message>
athrottle and concurrency config
</commit_message>
<xml_diff>
--- a/config/Metrics.xlsx
+++ b/config/Metrics.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\john\projects\appstorestream\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B79520-961C-4B19-920C-F1370F882F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811604F1-8B65-4BEC-BC01-CC4A22B69D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38925" yWindow="-16200" windowWidth="19200" windowHeight="16200" xr2:uid="{94CA47AB-981B-4FE4-B978-11EBD123BDAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="75945" windowHeight="21840" activeTab="1" xr2:uid="{94CA47AB-981B-4FE4-B978-11EBD123BDAA}"/>
   </bookViews>
   <sheets>
-    <sheet name="metrics" sheetId="1" r:id="rId1"/>
-    <sheet name="subcategory" sheetId="4" r:id="rId2"/>
-    <sheet name="category" sheetId="2" r:id="rId3"/>
-    <sheet name="levels" sheetId="3" r:id="rId4"/>
+    <sheet name="metrics (2)" sheetId="5" r:id="rId1"/>
+    <sheet name="metrics" sheetId="1" r:id="rId2"/>
+    <sheet name="subcategory" sheetId="4" r:id="rId3"/>
+    <sheet name="category" sheetId="2" r:id="rId4"/>
+    <sheet name="levels" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metrics!$A$1:$Y$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">metrics!$A$1:$Q$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'metrics (2)'!$A$1:$Y$73</definedName>
     <definedName name="categories">category!$A:$B</definedName>
     <definedName name="groups">category!$A:$A</definedName>
     <definedName name="labels">category!$G$1:$H$3</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="197">
   <si>
     <t>#</t>
   </si>
@@ -490,6 +492,144 @@
   </si>
   <si>
     <t>dataclass init</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract session  response latency total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract session average response size in bytes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract session total response size in bytes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract session retry count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract session error count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Client Error Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Server Error Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Redirect Error Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Unknown Error Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Errors / Requests </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session 1 - Failure_Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Average Latency / (Duration / Requests) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Average Latency / Average Duration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extract Session Total Latency  / Total Duration </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Start Timestamp In Seconds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Stop Timestamp In Seconds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Duration In Seconds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Record Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Record Size In Bytes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Records Processed Per Second  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Data Errors Encountered During Task </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Data Errors / Records </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform 1 - Failure_Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Start Timestamp In Seconds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Stop Timestamp In Seconds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Duration In Seconds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Load Record Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Total Load Record Count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Records Per Second </t>
+  </si>
+  <si>
+    <t>Histogram</t>
+  </si>
+  <si>
+    <t>Async HTTP request latency</t>
+  </si>
+  <si>
+    <t>HTTP Request Count</t>
+  </si>
+  <si>
+    <t>HTTP Request Latency</t>
+  </si>
+  <si>
+    <t>Failed HTTP Request Count</t>
+  </si>
+  <si>
+    <t>request_latency</t>
+  </si>
+  <si>
+    <t>response_size</t>
+  </si>
+  <si>
+    <t>Total of HTTP Response Sizes</t>
+  </si>
+  <si>
+    <t>http_requests</t>
+  </si>
+  <si>
+    <t>failed_http_requests</t>
+  </si>
+  <si>
+    <t>http_request_retries</t>
+  </si>
+  <si>
+    <t>HTTP Request Retries</t>
+  </si>
+  <si>
+    <t>sessions</t>
+  </si>
+  <si>
+    <t>Async HTTP Request Session Count</t>
+  </si>
+  <si>
+    <t>session_duration</t>
+  </si>
+  <si>
+    <t>Duration of Async HTTP Request Sessions</t>
+  </si>
+  <si>
+    <t>session_requests</t>
   </si>
 </sst>
 </file>
@@ -842,11 +982,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43C8825-BC9F-4D51-BF92-E4F675AB5ACF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B244B77-100E-48BE-B8EA-607E3EDE4A40}">
   <dimension ref="A1:Y73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,11 +1091,11 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:A33" si="0">VLOOKUP(F2,categories,2,FALSE)</f>
+        <f t="shared" ref="A2:A65" si="0">VLOOKUP(F2,categories,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B33" si="1">VLOOKUP(J2,subcategory,2,FALSE)</f>
+        <f t="shared" ref="B2:B65" si="1">VLOOKUP(J2,subcategory,2,FALSE)</f>
         <v>1</v>
       </c>
       <c r="C2">
@@ -983,21 +1123,21 @@
         <v>1</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="K2:K33" si="2">IF(J2="","","_")</f>
+        <f t="shared" ref="K2:K65" si="2">IF(J2="","","_")</f>
         <v>_</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M33" si="3">IF(N2="","","_")</f>
+        <f t="shared" ref="M2:M65" si="3">IF(N2="","","_")</f>
         <v>_</v>
       </c>
       <c r="N2" t="s">
         <v>27</v>
       </c>
       <c r="O2" t="str">
-        <f t="shared" ref="O2:O33" si="4">CONCATENATE(D2,E2,F2,G2,H2,I2,J2, K2,L2,M2,N2)</f>
+        <f t="shared" ref="O2:O65" si="4">CONCATENATE(D2,E2,F2,G2,H2,I2,J2, K2,L2,M2,N2)</f>
         <v>appstorestream_extract_job_runtime_start_timestamp_seconds</v>
       </c>
       <c r="P2" t="s">
@@ -1010,14 +1150,14 @@
         <v>68</v>
       </c>
       <c r="S2" t="str">
-        <f t="shared" ref="S2:S33" si="5">CONCATENATE(F2,G2,H2,I2,J2,K2,L2,M2,N2)</f>
+        <f t="shared" ref="S2:S65" si="5">CONCATENATE(F2,G2,H2,I2,J2,K2,L2,M2,N2)</f>
         <v>extract_job_runtime_start_timestamp_seconds</v>
       </c>
       <c r="T2" t="s">
         <v>46</v>
       </c>
       <c r="U2" t="str">
-        <f t="shared" ref="U2:U33" si="6">IF(T2="float"," = 0.0"," = 0")</f>
+        <f t="shared" ref="U2:U65" si="6">IF(T2="float"," = 0.0"," = 0")</f>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V2" t="str">
@@ -1032,7 +1172,7 @@
         <v>62</v>
       </c>
       <c r="Y2" t="str">
-        <f t="shared" ref="Y2:Y33" si="7">CONCATENATE("self.",O2,".labels(**self._labels).",X2,"(metrics.get('",S2,"',",0,"))")</f>
+        <f t="shared" ref="Y2:Y65" si="7">CONCATENATE("self.",O2,".labels(**self._labels).",X2,"(metrics.get('",S2,"',",0,"))")</f>
         <v>self.appstorestream_extract_job_runtime_start_timestamp_seconds.labels(**self._labels).set(metrics.get('extract_job_runtime_start_timestamp_seconds',0))</v>
       </c>
     </row>
@@ -1112,7 +1252,7 @@
         <v>runtime_stop_timestamp_seconds</v>
       </c>
       <c r="W3" t="str">
-        <f t="shared" ref="W3:W67" si="9">CONCATENATE(V3,": ",T3,U3)</f>
+        <f t="shared" ref="W3:W66" si="9">CONCATENATE(V3,": ",T3,U3)</f>
         <v>runtime_stop_timestamp_seconds: float = 0.0</v>
       </c>
       <c r="X3" t="s">
@@ -3735,11 +3875,11 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" ref="A34:A66" si="10">VLOOKUP(F34,categories,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B34">
-        <f t="shared" ref="B34:B66" si="11">VLOOKUP(J34,subcategory,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C34">
@@ -3767,21 +3907,21 @@
         <v>36</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" ref="K34:K66" si="12">IF(J34="","","_")</f>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L34" t="s">
         <v>31</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" ref="M34:M66" si="13">IF(N34="","","_")</f>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N34" t="s">
         <v>19</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" ref="O34:O66" si="14">CONCATENATE(D34,E34,F34,G34,H34,I34,J34, K34,L34,M34,N34)</f>
+        <f t="shared" si="4"/>
         <v>appstorestream_extract_task_success_failure_unknown_errors_total</v>
       </c>
       <c r="P34" t="s">
@@ -3794,14 +3934,14 @@
         <v>68</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" ref="S34:S68" si="15">CONCATENATE(F34,G34,H34,I34,J34,K34,L34,M34,N34)</f>
+        <f t="shared" si="5"/>
         <v>extract_task_success_failure_unknown_errors_total</v>
       </c>
       <c r="T34" t="s">
         <v>47</v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" ref="U34:U66" si="16">IF(T34="float"," = 0.0"," = 0")</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V34" t="str">
@@ -3816,17 +3956,17 @@
         <v>62</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" ref="Y34:Y66" si="17">CONCATENATE("self.",O34,".labels(**self._labels).",X34,"(metrics.get('",S34,"',",0,"))")</f>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_extract_task_success_failure_unknown_errors_total.labels(**self._labels).set(metrics.get('extract_task_success_failure_unknown_errors_total',0))</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C35">
@@ -3854,21 +3994,21 @@
         <v>36</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L35" t="s">
         <v>42</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N35" t="s">
         <v>16</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_extract_task_success_failure_request_failure_rate_ratio</v>
       </c>
       <c r="P35" t="s">
@@ -3881,14 +4021,14 @@
         <v>68</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>extract_task_success_failure_request_failure_rate_ratio</v>
       </c>
       <c r="T35" t="s">
         <v>46</v>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V35" t="str">
@@ -3903,17 +4043,17 @@
         <v>62</v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_extract_task_success_failure_request_failure_rate_ratio.labels(**self._labels).set(metrics.get('extract_task_success_failure_request_failure_rate_ratio',0))</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C36">
@@ -3941,21 +4081,21 @@
         <v>36</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L36" t="s">
         <v>41</v>
       </c>
       <c r="M36" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N36" t="s">
         <v>16</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_extract_task_success_failure_request_success_rate_ratio</v>
       </c>
       <c r="P36" t="s">
@@ -3968,14 +4108,14 @@
         <v>68</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>extract_task_success_failure_request_success_rate_ratio</v>
       </c>
       <c r="T36" t="s">
         <v>46</v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V36" t="str">
@@ -3990,17 +4130,17 @@
         <v>62</v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_extract_task_success_failure_request_success_rate_ratio.labels(**self._labels).set(metrics.get('extract_task_success_failure_request_success_rate_ratio',0))</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C37">
@@ -4028,21 +4168,21 @@
         <v>32</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L37" t="s">
         <v>21</v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N37" t="s">
         <v>16</v>
       </c>
       <c r="O37" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_extract_task_throttle_concurrency_efficiency_ratio</v>
       </c>
       <c r="P37" t="s">
@@ -4055,14 +4195,14 @@
         <v>68</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>extract_task_throttle_concurrency_efficiency_ratio</v>
       </c>
       <c r="T37" t="s">
         <v>46</v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V37" t="str">
@@ -4077,17 +4217,17 @@
         <v>62</v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_extract_task_throttle_concurrency_efficiency_ratio.labels(**self._labels).set(metrics.get('extract_task_throttle_concurrency_efficiency_ratio',0))</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C38">
@@ -4115,21 +4255,21 @@
         <v>32</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L38" t="s">
         <v>25</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N38" t="s">
         <v>16</v>
       </c>
       <c r="O38" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_extract_task_throttle_average_latency_efficiency_ratio</v>
       </c>
       <c r="P38" t="s">
@@ -4142,14 +4282,14 @@
         <v>68</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>extract_task_throttle_average_latency_efficiency_ratio</v>
       </c>
       <c r="T38" t="s">
         <v>46</v>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V38" t="str">
@@ -4164,17 +4304,17 @@
         <v>62</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_extract_task_throttle_average_latency_efficiency_ratio.labels(**self._labels).set(metrics.get('extract_task_throttle_average_latency_efficiency_ratio',0))</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C39">
@@ -4202,21 +4342,21 @@
         <v>32</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L39" t="s">
         <v>26</v>
       </c>
       <c r="M39" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N39" t="s">
         <v>16</v>
       </c>
       <c r="O39" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_extract_task_throttle_total_latency_efficiency_ratio</v>
       </c>
       <c r="P39" t="s">
@@ -4229,14 +4369,14 @@
         <v>68</v>
       </c>
       <c r="S39" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>extract_task_throttle_total_latency_efficiency_ratio</v>
       </c>
       <c r="T39" t="s">
         <v>46</v>
       </c>
       <c r="U39" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V39" t="str">
@@ -4251,17 +4391,17 @@
         <v>62</v>
       </c>
       <c r="Y39" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_extract_task_throttle_total_latency_efficiency_ratio.labels(**self._labels).set(metrics.get('extract_task_throttle_total_latency_efficiency_ratio',0))</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C40">
@@ -4289,21 +4429,21 @@
         <v>1</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L40" t="s">
         <v>12</v>
       </c>
       <c r="M40" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N40" t="s">
         <v>18</v>
       </c>
       <c r="O40" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_job_runtime_duration_seconds_total</v>
       </c>
       <c r="P40" t="s">
@@ -4316,14 +4456,14 @@
         <v>69</v>
       </c>
       <c r="S40" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_job_runtime_duration_seconds_total</v>
       </c>
       <c r="T40" t="s">
         <v>46</v>
       </c>
       <c r="U40" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V40" t="str">
@@ -4338,17 +4478,17 @@
         <v>64</v>
       </c>
       <c r="Y40" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_job_runtime_duration_seconds_total.labels(**self._labels).inc(metrics.get('transform_job_runtime_duration_seconds_total',0))</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C41">
@@ -4376,21 +4516,21 @@
         <v>72</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L41" t="s">
         <v>71</v>
       </c>
       <c r="M41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N41" t="s">
         <v>19</v>
       </c>
       <c r="O41" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_job_record_count_total</v>
       </c>
       <c r="P41" t="s">
@@ -4403,14 +4543,14 @@
         <v>69</v>
       </c>
       <c r="S41" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_job_record_count_total</v>
       </c>
       <c r="T41" t="s">
         <v>47</v>
       </c>
       <c r="U41" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V41" t="str">
@@ -4425,17 +4565,17 @@
         <v>64</v>
       </c>
       <c r="Y41" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_job_record_count_total.labels(**self._labels).inc(metrics.get('transform_job_record_count_total',0))</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C42">
@@ -4463,21 +4603,21 @@
         <v>72</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L42" t="s">
         <v>57</v>
       </c>
       <c r="M42" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N42" t="s">
         <v>51</v>
       </c>
       <c r="O42" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_job_record_size_bytes_total</v>
       </c>
       <c r="P42" t="s">
@@ -4490,14 +4630,14 @@
         <v>69</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_job_record_size_bytes_total</v>
       </c>
       <c r="T42" t="s">
         <v>47</v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V42" t="str">
@@ -4512,17 +4652,17 @@
         <v>64</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_job_record_size_bytes_total.labels(**self._labels).inc(metrics.get('transform_job_record_size_bytes_total',0))</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B43">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C43">
@@ -4550,21 +4690,21 @@
         <v>72</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L43" t="s">
         <v>39</v>
       </c>
       <c r="M43" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N43" t="s">
         <v>16</v>
       </c>
       <c r="O43" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_job_record_per_second_ratio</v>
       </c>
       <c r="P43" t="s">
@@ -4577,14 +4717,14 @@
         <v>69</v>
       </c>
       <c r="S43" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_job_record_per_second_ratio</v>
       </c>
       <c r="T43" t="s">
         <v>46</v>
       </c>
       <c r="U43" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V43" t="str">
@@ -4599,17 +4739,17 @@
         <v>62</v>
       </c>
       <c r="Y43" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_job_record_per_second_ratio.labels(**self._labels).set(metrics.get('transform_job_record_per_second_ratio',0))</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C44">
@@ -4637,21 +4777,21 @@
         <v>36</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L44" t="s">
         <v>4</v>
       </c>
       <c r="M44" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N44" t="s">
         <v>19</v>
       </c>
       <c r="O44" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_job_success_failure_data_errors_total</v>
       </c>
       <c r="P44" t="s">
@@ -4664,14 +4804,14 @@
         <v>69</v>
       </c>
       <c r="S44" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_job_success_failure_data_errors_total</v>
       </c>
       <c r="T44" t="s">
         <v>47</v>
       </c>
       <c r="U44" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V44" t="str">
@@ -4686,17 +4826,17 @@
         <v>64</v>
       </c>
       <c r="Y44" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_job_success_failure_data_errors_total.labels(**self._labels).inc(metrics.get('transform_job_success_failure_data_errors_total',0))</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C45">
@@ -4724,21 +4864,21 @@
         <v>36</v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L45" t="s">
         <v>9</v>
       </c>
       <c r="M45" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N45" t="s">
         <v>16</v>
       </c>
       <c r="O45" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_job_success_failure_data_error_rate_ratio</v>
       </c>
       <c r="P45" t="s">
@@ -4751,14 +4891,14 @@
         <v>69</v>
       </c>
       <c r="S45" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_job_success_failure_data_error_rate_ratio</v>
       </c>
       <c r="T45" t="s">
         <v>47</v>
       </c>
       <c r="U45" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V45" t="str">
@@ -4773,17 +4913,17 @@
         <v>62</v>
       </c>
       <c r="Y45" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_job_success_failure_data_error_rate_ratio.labels(**self._labels).set(metrics.get('transform_job_success_failure_data_error_rate_ratio',0))</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B46">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C46">
@@ -4811,21 +4951,21 @@
         <v>36</v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L46" t="s">
         <v>77</v>
       </c>
       <c r="M46" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N46" t="s">
         <v>16</v>
       </c>
       <c r="O46" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_job_success_failure_record_success_rate_ratio</v>
       </c>
       <c r="P46" t="s">
@@ -4838,14 +4978,14 @@
         <v>69</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_job_success_failure_record_success_rate_ratio</v>
       </c>
       <c r="T46" t="s">
         <v>46</v>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V46" t="str">
@@ -4860,17 +5000,17 @@
         <v>62</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_job_success_failure_record_success_rate_ratio.labels(**self._labels).set(metrics.get('transform_job_success_failure_record_success_rate_ratio',0))</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B47">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C47">
@@ -4898,21 +5038,21 @@
         <v>1</v>
       </c>
       <c r="K47" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L47" t="s">
         <v>28</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N47" t="s">
         <v>27</v>
       </c>
       <c r="O47" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_runtime_start_timestamp_seconds</v>
       </c>
       <c r="P47" t="s">
@@ -4925,14 +5065,14 @@
         <v>69</v>
       </c>
       <c r="S47" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_runtime_start_timestamp_seconds</v>
       </c>
       <c r="T47" t="s">
         <v>46</v>
       </c>
       <c r="U47" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V47" t="str">
@@ -4947,17 +5087,17 @@
         <v>62</v>
       </c>
       <c r="Y47" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_runtime_start_timestamp_seconds.labels(**self._labels).set(metrics.get('transform_task_runtime_start_timestamp_seconds',0))</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C48">
@@ -4985,21 +5125,21 @@
         <v>1</v>
       </c>
       <c r="K48" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L48" t="s">
         <v>40</v>
       </c>
       <c r="M48" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N48" t="s">
         <v>27</v>
       </c>
       <c r="O48" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_runtime_stop_timestamp_seconds</v>
       </c>
       <c r="P48" t="s">
@@ -5012,14 +5152,14 @@
         <v>69</v>
       </c>
       <c r="S48" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_runtime_stop_timestamp_seconds</v>
       </c>
       <c r="T48" t="s">
         <v>46</v>
       </c>
       <c r="U48" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V48" t="str">
@@ -5034,17 +5174,17 @@
         <v>62</v>
       </c>
       <c r="Y48" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_runtime_stop_timestamp_seconds.labels(**self._labels).set(metrics.get('transform_task_runtime_stop_timestamp_seconds',0))</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C49">
@@ -5072,21 +5212,21 @@
         <v>1</v>
       </c>
       <c r="K49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L49" t="s">
         <v>12</v>
       </c>
       <c r="M49" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N49" t="s">
         <v>15</v>
       </c>
       <c r="O49" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_runtime_duration_seconds</v>
       </c>
       <c r="P49" t="s">
@@ -5099,14 +5239,14 @@
         <v>69</v>
       </c>
       <c r="S49" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_runtime_duration_seconds</v>
       </c>
       <c r="T49" t="s">
         <v>46</v>
       </c>
       <c r="U49" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V49" t="str">
@@ -5121,17 +5261,17 @@
         <v>62</v>
       </c>
       <c r="Y49" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_runtime_duration_seconds.labels(**self._labels).set(metrics.get('transform_task_runtime_duration_seconds',0))</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C50">
@@ -5159,18 +5299,18 @@
         <v>72</v>
       </c>
       <c r="K50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L50" t="s">
         <v>71</v>
       </c>
       <c r="M50" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O50" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_record_count</v>
       </c>
       <c r="P50" t="s">
@@ -5183,14 +5323,14 @@
         <v>69</v>
       </c>
       <c r="S50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_record_count</v>
       </c>
       <c r="T50" t="s">
         <v>47</v>
       </c>
       <c r="U50" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V50" t="str">
@@ -5205,17 +5345,17 @@
         <v>62</v>
       </c>
       <c r="Y50" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_record_count.labels(**self._labels).set(metrics.get('transform_task_record_count',0))</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" ref="A51" si="18">VLOOKUP(F51,categories,2,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B51">
-        <f t="shared" ref="B51" si="19">VLOOKUP(J51,subcategory,2,FALSE)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C51">
@@ -5243,21 +5383,21 @@
         <v>72</v>
       </c>
       <c r="K51" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L51" t="s">
         <v>57</v>
       </c>
       <c r="M51" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N51" t="s">
         <v>51</v>
       </c>
       <c r="O51" t="str">
-        <f t="shared" ref="O51" si="20">CONCATENATE(D51,E51,F51,G51,H51,I51,J51, K51,L51,M51,N51)</f>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_record_size_bytes_total</v>
       </c>
       <c r="P51" t="s">
@@ -5270,39 +5410,39 @@
         <v>69</v>
       </c>
       <c r="S51" t="str">
-        <f t="shared" ref="S51" si="21">CONCATENATE(F51,G51,H51,I51,J51,K51,L51,M51,N51)</f>
+        <f t="shared" si="5"/>
         <v>transform_task_record_size_bytes_total</v>
       </c>
       <c r="T51" t="s">
         <v>47</v>
       </c>
       <c r="U51" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V51" t="str">
-        <f t="shared" ref="V51" si="22">CONCATENATE(J51,K51,L51,M51,N51)</f>
+        <f t="shared" si="8"/>
         <v>record_size_bytes_total</v>
       </c>
       <c r="W51" t="str">
-        <f t="shared" ref="W51" si="23">CONCATENATE(V51,": ",T51,U51)</f>
+        <f t="shared" si="9"/>
         <v>record_size_bytes_total: int = 0</v>
       </c>
       <c r="X51" t="s">
         <v>62</v>
       </c>
       <c r="Y51" t="str">
-        <f t="shared" ref="Y51" si="24">CONCATENATE("self.",O51,".labels(**self._labels).",X51,"(metrics.get('",S51,"',",0,"))")</f>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_record_size_bytes_total.labels(**self._labels).set(metrics.get('transform_task_record_size_bytes_total',0))</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B52">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C52">
@@ -5330,21 +5470,21 @@
         <v>72</v>
       </c>
       <c r="K52" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L52" t="s">
         <v>61</v>
       </c>
       <c r="M52" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N52" t="s">
         <v>35</v>
       </c>
       <c r="O52" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_record_average_size_bytes</v>
       </c>
       <c r="P52" t="s">
@@ -5357,14 +5497,14 @@
         <v>69</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_record_average_size_bytes</v>
       </c>
       <c r="T52" t="s">
         <v>47</v>
       </c>
       <c r="U52" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V52" t="str">
@@ -5379,17 +5519,17 @@
         <v>62</v>
       </c>
       <c r="Y52" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_record_average_size_bytes.labels(**self._labels).set(metrics.get('transform_task_record_average_size_bytes',0))</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B53">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C53">
@@ -5417,21 +5557,21 @@
         <v>72</v>
       </c>
       <c r="K53" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L53" t="s">
         <v>39</v>
       </c>
       <c r="M53" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N53" t="s">
         <v>16</v>
       </c>
       <c r="O53" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_record_per_second_ratio</v>
       </c>
       <c r="P53" t="s">
@@ -5444,14 +5584,14 @@
         <v>69</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_record_per_second_ratio</v>
       </c>
       <c r="T53" t="s">
         <v>46</v>
       </c>
       <c r="U53" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V53" t="str">
@@ -5466,17 +5606,17 @@
         <v>62</v>
       </c>
       <c r="Y53" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_record_per_second_ratio.labels(**self._labels).set(metrics.get('transform_task_record_per_second_ratio',0))</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B54">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C54">
@@ -5504,21 +5644,21 @@
         <v>36</v>
       </c>
       <c r="K54" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L54" t="s">
         <v>4</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N54" t="s">
         <v>19</v>
       </c>
       <c r="O54" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_success_failure_data_errors_total</v>
       </c>
       <c r="P54" t="s">
@@ -5531,14 +5671,14 @@
         <v>69</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_success_failure_data_errors_total</v>
       </c>
       <c r="T54" t="s">
         <v>47</v>
       </c>
       <c r="U54" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V54" t="str">
@@ -5553,17 +5693,17 @@
         <v>62</v>
       </c>
       <c r="Y54" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_success_failure_data_errors_total.labels(**self._labels).set(metrics.get('transform_task_success_failure_data_errors_total',0))</v>
       </c>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B55">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C55">
@@ -5591,21 +5731,21 @@
         <v>36</v>
       </c>
       <c r="K55" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L55" t="s">
         <v>9</v>
       </c>
       <c r="M55" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N55" t="s">
         <v>16</v>
       </c>
       <c r="O55" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_success_failure_data_error_rate_ratio</v>
       </c>
       <c r="P55" t="s">
@@ -5618,14 +5758,14 @@
         <v>69</v>
       </c>
       <c r="S55" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_success_failure_data_error_rate_ratio</v>
       </c>
       <c r="T55" t="s">
         <v>47</v>
       </c>
       <c r="U55" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V55" t="str">
@@ -5640,17 +5780,17 @@
         <v>62</v>
       </c>
       <c r="Y55" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_success_failure_data_error_rate_ratio.labels(**self._labels).set(metrics.get('transform_task_success_failure_data_error_rate_ratio',0))</v>
       </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C56">
@@ -5678,21 +5818,21 @@
         <v>36</v>
       </c>
       <c r="K56" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L56" t="s">
         <v>77</v>
       </c>
       <c r="M56" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N56" t="s">
         <v>16</v>
       </c>
       <c r="O56" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_transform_task_success_failure_record_success_rate_ratio</v>
       </c>
       <c r="P56" t="s">
@@ -5705,14 +5845,14 @@
         <v>69</v>
       </c>
       <c r="S56" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>transform_task_success_failure_record_success_rate_ratio</v>
       </c>
       <c r="T56" t="s">
         <v>46</v>
       </c>
       <c r="U56" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V56" t="str">
@@ -5727,17 +5867,17 @@
         <v>62</v>
       </c>
       <c r="Y56" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_transform_task_success_failure_record_success_rate_ratio.labels(**self._labels).set(metrics.get('transform_task_success_failure_record_success_rate_ratio',0))</v>
       </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B57">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C57">
@@ -5765,21 +5905,21 @@
         <v>1</v>
       </c>
       <c r="K57" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L57" t="s">
         <v>12</v>
       </c>
       <c r="M57" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N57" t="s">
         <v>18</v>
       </c>
       <c r="O57" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_job_runtime_duration_seconds_total</v>
       </c>
       <c r="P57" t="s">
@@ -5792,14 +5932,14 @@
         <v>70</v>
       </c>
       <c r="S57" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_job_runtime_duration_seconds_total</v>
       </c>
       <c r="T57" t="s">
         <v>46</v>
       </c>
       <c r="U57" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V57" t="str">
@@ -5814,17 +5954,17 @@
         <v>64</v>
       </c>
       <c r="Y57" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_job_runtime_duration_seconds_total.labels(**self._labels).inc(metrics.get('load_job_runtime_duration_seconds_total',0))</v>
       </c>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C58">
@@ -5852,21 +5992,21 @@
         <v>72</v>
       </c>
       <c r="K58" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L58" t="s">
         <v>71</v>
       </c>
       <c r="M58" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N58" t="s">
         <v>19</v>
       </c>
       <c r="O58" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_job_record_count_total</v>
       </c>
       <c r="P58" t="s">
@@ -5879,14 +6019,14 @@
         <v>70</v>
       </c>
       <c r="S58" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_job_record_count_total</v>
       </c>
       <c r="T58" t="s">
         <v>47</v>
       </c>
       <c r="U58" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V58" t="str">
@@ -5901,17 +6041,17 @@
         <v>64</v>
       </c>
       <c r="Y58" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_job_record_count_total.labels(**self._labels).inc(metrics.get('load_job_record_count_total',0))</v>
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C59">
@@ -5939,21 +6079,21 @@
         <v>72</v>
       </c>
       <c r="K59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L59" t="s">
         <v>61</v>
       </c>
       <c r="M59" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N59" t="s">
         <v>35</v>
       </c>
       <c r="O59" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_job_record_average_size_bytes</v>
       </c>
       <c r="P59" t="s">
@@ -5966,14 +6106,14 @@
         <v>70</v>
       </c>
       <c r="S59" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_job_record_average_size_bytes</v>
       </c>
       <c r="T59" t="s">
         <v>47</v>
       </c>
       <c r="U59" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V59" t="str">
@@ -5988,17 +6128,17 @@
         <v>62</v>
       </c>
       <c r="Y59" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_job_record_average_size_bytes.labels(**self._labels).set(metrics.get('load_job_record_average_size_bytes',0))</v>
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C60">
@@ -6026,21 +6166,21 @@
         <v>72</v>
       </c>
       <c r="K60" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L60" t="s">
         <v>57</v>
       </c>
       <c r="M60" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N60" t="s">
         <v>51</v>
       </c>
       <c r="O60" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_job_record_size_bytes_total</v>
       </c>
       <c r="P60" t="s">
@@ -6053,14 +6193,14 @@
         <v>70</v>
       </c>
       <c r="S60" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_job_record_size_bytes_total</v>
       </c>
       <c r="T60" t="s">
         <v>47</v>
       </c>
       <c r="U60" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V60" t="str">
@@ -6075,17 +6215,17 @@
         <v>64</v>
       </c>
       <c r="Y60" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_job_record_size_bytes_total.labels(**self._labels).inc(metrics.get('load_job_record_size_bytes_total',0))</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C61">
@@ -6113,21 +6253,21 @@
         <v>72</v>
       </c>
       <c r="K61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L61" t="s">
         <v>39</v>
       </c>
       <c r="M61" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N61" t="s">
         <v>16</v>
       </c>
       <c r="O61" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_job_record_per_second_ratio</v>
       </c>
       <c r="P61" t="s">
@@ -6140,14 +6280,14 @@
         <v>70</v>
       </c>
       <c r="S61" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_job_record_per_second_ratio</v>
       </c>
       <c r="T61" t="s">
         <v>46</v>
       </c>
       <c r="U61" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V61" t="str">
@@ -6162,17 +6302,17 @@
         <v>62</v>
       </c>
       <c r="Y61" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_job_record_per_second_ratio.labels(**self._labels).set(metrics.get('load_job_record_per_second_ratio',0))</v>
       </c>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C62">
@@ -6200,21 +6340,21 @@
         <v>1</v>
       </c>
       <c r="K62" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L62" t="s">
         <v>28</v>
       </c>
       <c r="M62" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N62" t="s">
         <v>27</v>
       </c>
       <c r="O62" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_task_runtime_start_timestamp_seconds</v>
       </c>
       <c r="P62" t="s">
@@ -6227,14 +6367,14 @@
         <v>70</v>
       </c>
       <c r="S62" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_task_runtime_start_timestamp_seconds</v>
       </c>
       <c r="T62" t="s">
         <v>46</v>
       </c>
       <c r="U62" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V62" t="str">
@@ -6249,17 +6389,17 @@
         <v>62</v>
       </c>
       <c r="Y62" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_task_runtime_start_timestamp_seconds.labels(**self._labels).set(metrics.get('load_task_runtime_start_timestamp_seconds',0))</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C63">
@@ -6287,21 +6427,21 @@
         <v>1</v>
       </c>
       <c r="K63" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L63" t="s">
         <v>40</v>
       </c>
       <c r="M63" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N63" t="s">
         <v>27</v>
       </c>
       <c r="O63" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_task_runtime_stop_timestamp_seconds</v>
       </c>
       <c r="P63" t="s">
@@ -6314,14 +6454,14 @@
         <v>70</v>
       </c>
       <c r="S63" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_task_runtime_stop_timestamp_seconds</v>
       </c>
       <c r="T63" t="s">
         <v>46</v>
       </c>
       <c r="U63" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V63" t="str">
@@ -6336,17 +6476,17 @@
         <v>62</v>
       </c>
       <c r="Y63" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_task_runtime_stop_timestamp_seconds.labels(**self._labels).set(metrics.get('load_task_runtime_stop_timestamp_seconds',0))</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B64">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C64">
@@ -6374,21 +6514,21 @@
         <v>1</v>
       </c>
       <c r="K64" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L64" t="s">
         <v>12</v>
       </c>
       <c r="M64" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v>_</v>
       </c>
       <c r="N64" t="s">
         <v>15</v>
       </c>
       <c r="O64" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_task_runtime_duration_seconds</v>
       </c>
       <c r="P64" t="s">
@@ -6401,14 +6541,14 @@
         <v>70</v>
       </c>
       <c r="S64" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_task_runtime_duration_seconds</v>
       </c>
       <c r="T64" t="s">
         <v>46</v>
       </c>
       <c r="U64" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V64" t="str">
@@ -6423,17 +6563,17 @@
         <v>62</v>
       </c>
       <c r="Y64" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_task_runtime_duration_seconds.labels(**self._labels).set(metrics.get('load_task_runtime_duration_seconds',0))</v>
       </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C65">
@@ -6461,18 +6601,18 @@
         <v>72</v>
       </c>
       <c r="K65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>_</v>
       </c>
       <c r="L65" t="s">
         <v>71</v>
       </c>
       <c r="M65" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O65" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="4"/>
         <v>appstorestream_load_task_record_count</v>
       </c>
       <c r="P65" t="s">
@@ -6485,14 +6625,14 @@
         <v>70</v>
       </c>
       <c r="S65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="5"/>
         <v>load_task_record_count</v>
       </c>
       <c r="T65" t="s">
         <v>47</v>
       </c>
       <c r="U65" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V65" t="str">
@@ -6507,17 +6647,17 @@
         <v>62</v>
       </c>
       <c r="Y65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="7"/>
         <v>self.appstorestream_load_task_record_count.labels(**self._labels).set(metrics.get('load_task_record_count',0))</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="A66:A73" si="10">VLOOKUP(F66,categories,2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="B66">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="B66:B73" si="11">VLOOKUP(J66,subcategory,2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="C66">
@@ -6545,21 +6685,21 @@
         <v>72</v>
       </c>
       <c r="K66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="K66:K73" si="12">IF(J66="","","_")</f>
         <v>_</v>
       </c>
       <c r="L66" t="s">
         <v>61</v>
       </c>
       <c r="M66" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="M66:M73" si="13">IF(N66="","","_")</f>
         <v>_</v>
       </c>
       <c r="N66" t="s">
         <v>35</v>
       </c>
       <c r="O66" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="O66:O73" si="14">CONCATENATE(D66,E66,F66,G66,H66,I66,J66, K66,L66,M66,N66)</f>
         <v>appstorestream_load_task_record_average_size_bytes</v>
       </c>
       <c r="P66" t="s">
@@ -6572,14 +6712,14 @@
         <v>70</v>
       </c>
       <c r="S66" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="S66:S73" si="15">CONCATENATE(F66,G66,H66,I66,J66,K66,L66,M66,N66)</f>
         <v>load_task_record_average_size_bytes</v>
       </c>
       <c r="T66" t="s">
         <v>47</v>
       </c>
       <c r="U66" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="U66:U73" si="16">IF(T66="float"," = 0.0"," = 0")</f>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V66" t="str">
@@ -6594,17 +6734,17 @@
         <v>62</v>
       </c>
       <c r="Y66" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="Y66:Y73" si="17">CONCATENATE("self.",O66,".labels(**self._labels).",X66,"(metrics.get('",S66,"',",0,"))")</f>
         <v>self.appstorestream_load_task_record_average_size_bytes.labels(**self._labels).set(metrics.get('load_task_record_average_size_bytes',0))</v>
       </c>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" ref="A67:A73" si="25">VLOOKUP(F67,categories,2,FALSE)</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B73" si="26">VLOOKUP(J67,subcategory,2,FALSE)</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="C67">
@@ -6632,21 +6772,21 @@
         <v>72</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K98" si="27">IF(J67="","","_")</f>
+        <f t="shared" si="12"/>
         <v>_</v>
       </c>
       <c r="L67" t="s">
         <v>57</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" ref="M67:M98" si="28">IF(N67="","","_")</f>
+        <f t="shared" si="13"/>
         <v>_</v>
       </c>
       <c r="N67" t="s">
         <v>51</v>
       </c>
       <c r="O67" t="str">
-        <f t="shared" ref="O67:O98" si="29">CONCATENATE(D67,E67,F67,G67,H67,I67,J67, K67,L67,M67,N67)</f>
+        <f t="shared" si="14"/>
         <v>appstorestream_load_task_record_size_bytes_total</v>
       </c>
       <c r="P67" t="s">
@@ -6666,7 +6806,7 @@
         <v>47</v>
       </c>
       <c r="U67" t="str">
-        <f t="shared" ref="U67:U98" si="30">IF(T67="float"," = 0.0"," = 0")</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V67" t="str">
@@ -6674,24 +6814,24 @@
         <v>record_size_bytes_total</v>
       </c>
       <c r="W67" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="W67:W73" si="18">CONCATENATE(V67,": ",T67,U67)</f>
         <v>record_size_bytes_total: int = 0</v>
       </c>
       <c r="X67" t="s">
         <v>62</v>
       </c>
       <c r="Y67" t="str">
-        <f t="shared" ref="Y67:Y98" si="31">CONCATENATE("self.",O67,".labels(**self._labels).",X67,"(metrics.get('",S67,"',",0,"))")</f>
+        <f t="shared" si="17"/>
         <v>self.appstorestream_load_task_record_size_bytes_total.labels(**self._labels).set(metrics.get('load_task_record_size_bytes_total',0))</v>
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="25"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="B68">
-        <f t="shared" si="26"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="C68">
@@ -6719,21 +6859,21 @@
         <v>72</v>
       </c>
       <c r="K68" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>_</v>
       </c>
       <c r="L68" t="s">
         <v>39</v>
       </c>
       <c r="M68" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>_</v>
       </c>
       <c r="N68" t="s">
         <v>16</v>
       </c>
       <c r="O68" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>appstorestream_load_task_record_per_second_ratio</v>
       </c>
       <c r="P68" t="s">
@@ -6753,32 +6893,32 @@
         <v>46</v>
       </c>
       <c r="U68" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V68" t="str">
-        <f t="shared" ref="V68:V73" si="32">CONCATENATE(J68,K68,L68,M68,N68)</f>
+        <f t="shared" ref="V68:V73" si="19">CONCATENATE(J68,K68,L68,M68,N68)</f>
         <v>record_per_second_ratio</v>
       </c>
       <c r="W68" t="str">
-        <f t="shared" ref="W68:W73" si="33">CONCATENATE(V68,": ",T68,U68)</f>
+        <f t="shared" si="18"/>
         <v>record_per_second_ratio: float = 0.0</v>
       </c>
       <c r="X68" t="s">
         <v>62</v>
       </c>
       <c r="Y68" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="17"/>
         <v>self.appstorestream_load_task_record_per_second_ratio.labels(**self._labels).set(metrics.get('load_task_record_per_second_ratio',0))</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="25"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="B69">
-        <f t="shared" si="26"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="D69" t="s">
@@ -6803,21 +6943,21 @@
         <v>58</v>
       </c>
       <c r="K69" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>_</v>
       </c>
       <c r="L69" t="s">
         <v>48</v>
       </c>
       <c r="M69" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>_</v>
       </c>
       <c r="N69" t="s">
         <v>35</v>
       </c>
       <c r="O69" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>appstorestream_system_job_network_io_bytes</v>
       </c>
       <c r="P69" t="s">
@@ -6830,39 +6970,39 @@
         <v>49</v>
       </c>
       <c r="S69" t="str">
-        <f t="shared" ref="S69:S73" si="34">CONCATENATE(F69,G69,H69,I69,J69,K69,L69,M69,N69)</f>
+        <f t="shared" si="15"/>
         <v>system_job_network_io_bytes</v>
       </c>
       <c r="T69" t="s">
         <v>47</v>
       </c>
       <c r="U69" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V69" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="19"/>
         <v>network_io_bytes</v>
       </c>
       <c r="W69" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="18"/>
         <v>network_io_bytes: int = 0</v>
       </c>
       <c r="X69" t="s">
         <v>64</v>
       </c>
       <c r="Y69" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="17"/>
         <v>self.appstorestream_system_job_network_io_bytes.labels(**self._labels).inc(metrics.get('system_job_network_io_bytes',0))</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="25"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="B70">
-        <f t="shared" si="26"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="D70" t="s">
@@ -6887,21 +7027,21 @@
         <v>59</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>_</v>
       </c>
       <c r="L70" t="s">
         <v>48</v>
       </c>
       <c r="M70" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>_</v>
       </c>
       <c r="N70" t="s">
         <v>35</v>
       </c>
       <c r="O70" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>appstorestream_system_job_disk_io_bytes</v>
       </c>
       <c r="P70" t="s">
@@ -6914,39 +7054,39 @@
         <v>49</v>
       </c>
       <c r="S70" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>system_job_disk_io_bytes</v>
       </c>
       <c r="T70" t="s">
         <v>47</v>
       </c>
       <c r="U70" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V70" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="19"/>
         <v>disk_io_bytes</v>
       </c>
       <c r="W70" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="18"/>
         <v>disk_io_bytes: int = 0</v>
       </c>
       <c r="X70" t="s">
         <v>64</v>
       </c>
       <c r="Y70" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="17"/>
         <v>self.appstorestream_system_job_disk_io_bytes.labels(**self._labels).inc(metrics.get('system_job_disk_io_bytes',0))</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="25"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="B71">
-        <f t="shared" si="26"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="D71" t="s">
@@ -6971,21 +7111,21 @@
         <v>57</v>
       </c>
       <c r="K71" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>_</v>
       </c>
       <c r="L71" t="s">
         <v>60</v>
       </c>
       <c r="M71" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>_</v>
       </c>
       <c r="N71" t="s">
         <v>35</v>
       </c>
       <c r="O71" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>appstorestream_system_job_size_db_bytes</v>
       </c>
       <c r="P71" t="s">
@@ -6998,39 +7138,39 @@
         <v>49</v>
       </c>
       <c r="S71" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>system_job_size_db_bytes</v>
       </c>
       <c r="T71" t="s">
         <v>47</v>
       </c>
       <c r="U71" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> = 0</v>
       </c>
       <c r="V71" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="19"/>
         <v>size_db_bytes</v>
       </c>
       <c r="W71" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="18"/>
         <v>size_db_bytes: int = 0</v>
       </c>
       <c r="X71" t="s">
         <v>64</v>
       </c>
       <c r="Y71" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="17"/>
         <v>self.appstorestream_system_job_size_db_bytes.labels(**self._labels).inc(metrics.get('system_job_size_db_bytes',0))</v>
       </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="25"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="B72">
-        <f t="shared" si="26"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="D72" t="s">
@@ -7055,21 +7195,21 @@
         <v>34</v>
       </c>
       <c r="K72" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>_</v>
       </c>
       <c r="L72" t="s">
         <v>75</v>
       </c>
       <c r="M72" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>_</v>
       </c>
       <c r="N72" t="s">
         <v>16</v>
       </c>
       <c r="O72" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>appstorestream_system_job_cpu_average_pct_ratio</v>
       </c>
       <c r="P72" t="s">
@@ -7082,39 +7222,39 @@
         <v>49</v>
       </c>
       <c r="S72" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>system_job_cpu_average_pct_ratio</v>
       </c>
       <c r="T72" t="s">
         <v>46</v>
       </c>
       <c r="U72" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V72" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="19"/>
         <v>cpu_average_pct_ratio</v>
       </c>
       <c r="W72" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="18"/>
         <v>cpu_average_pct_ratio: float = 0.0</v>
       </c>
       <c r="X72" t="s">
         <v>62</v>
       </c>
       <c r="Y72" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="17"/>
         <v>self.appstorestream_system_job_cpu_average_pct_ratio.labels(**self._labels).set(metrics.get('system_job_cpu_average_pct_ratio',0))</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="25"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="B73">
-        <f t="shared" si="26"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="D73" t="s">
@@ -7139,21 +7279,21 @@
         <v>76</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="12"/>
         <v>_</v>
       </c>
       <c r="L73" t="s">
         <v>75</v>
       </c>
       <c r="M73" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="13"/>
         <v>_</v>
       </c>
       <c r="N73" t="s">
         <v>16</v>
       </c>
       <c r="O73" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="14"/>
         <v>appstorestream_system_job_memory_average_pct_ratio</v>
       </c>
       <c r="P73" t="s">
@@ -7166,45 +7306,1670 @@
         <v>49</v>
       </c>
       <c r="S73" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="15"/>
         <v>system_job_memory_average_pct_ratio</v>
       </c>
       <c r="T73" t="s">
         <v>46</v>
       </c>
       <c r="U73" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="16"/>
         <v xml:space="preserve"> = 0.0</v>
       </c>
       <c r="V73" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="19"/>
         <v>memory_average_pct_ratio</v>
       </c>
       <c r="W73" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="18"/>
         <v>memory_average_pct_ratio: float = 0.0</v>
       </c>
       <c r="X73" t="s">
         <v>62</v>
       </c>
       <c r="Y73" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="17"/>
         <v>self.appstorestream_system_job_memory_average_pct_ratio.labels(**self._labels).set(metrics.get('system_job_memory_average_pct_ratio',0))</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y73">
-    <sortCondition ref="A4:A73"/>
-    <sortCondition ref="H4:H73"/>
-    <sortCondition ref="B4:B73"/>
-    <sortCondition ref="C4:C73"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43C8825-BC9F-4D51-BF92-E4F675AB5ACF}">
+  <dimension ref="A1:J47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="65" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="52.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2" si="0">IF(C2="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" t="str">
+        <f>IF(G2="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE(A2,B2,E2,F2,G2)</f>
+        <v>appstorestream_http_requests_total</v>
+      </c>
+      <c r="I2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D19" si="1">IF(C3="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" t="str">
+        <f>IF(G3="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H47" si="2">CONCATENATE(A3,B3,E3,F3,G3)</f>
+        <v>appstorestream_failed_http_requests_total</v>
+      </c>
+      <c r="I3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F47" si="3">IF(G4="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_request_latency_seconds</v>
+      </c>
+      <c r="I4" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF(C5="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_response_size_bytes_total</v>
+      </c>
+      <c r="I5" t="s">
+        <v>187</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_http_request_retries</v>
+      </c>
+      <c r="I6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" ref="D7" si="4">IF(C7="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ref="H7" si="5">CONCATENATE(A7,B7,E7,F7,G7)</f>
+        <v>appstorestream_sessions_total</v>
+      </c>
+      <c r="I7" t="s">
+        <v>193</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" ref="D8" si="6">IF(C8="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" ref="H8" si="7">CONCATENATE(A8,B8,E8,F8,G8)</f>
+        <v>appstorestream_session_duration_seconds</v>
+      </c>
+      <c r="I8" t="s">
+        <v>195</v>
+      </c>
+      <c r="J8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" ref="D9" si="8">IF(C9="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" ref="H9" si="9">CONCATENATE(A9,B9,E9,F9,G9)</f>
+        <v>appstorestream_session_requests_seconds</v>
+      </c>
+      <c r="I9" t="s">
+        <v>195</v>
+      </c>
+      <c r="J9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_latency_seconds</v>
+      </c>
+      <c r="I11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_latency_seconds</v>
+      </c>
+      <c r="I12" t="s">
+        <v>151</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_average_size_bytes</v>
+      </c>
+      <c r="I13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_size_bytes_total</v>
+      </c>
+      <c r="I14" t="s">
+        <v>153</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_retries_total</v>
+      </c>
+      <c r="I15" t="s">
+        <v>154</v>
+      </c>
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_errors_total</v>
+      </c>
+      <c r="I16" t="s">
+        <v>155</v>
+      </c>
+      <c r="J16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_client_errors_total</v>
+      </c>
+      <c r="I17" t="s">
+        <v>156</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_server_errors_total</v>
+      </c>
+      <c r="I18" t="s">
+        <v>157</v>
+      </c>
+      <c r="J18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>_</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_redirect_errors_total</v>
+      </c>
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" ref="D20:D40" si="10">IF(C20="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_unknown_errors_total</v>
+      </c>
+      <c r="I20" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_request_failure_rate_ratio</v>
+      </c>
+      <c r="I21" t="s">
+        <v>160</v>
+      </c>
+      <c r="J21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_request_success_rate_ratio</v>
+      </c>
+      <c r="I22" t="s">
+        <v>161</v>
+      </c>
+      <c r="J22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_concurrency_efficiency_ratio</v>
+      </c>
+      <c r="I23" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_average_latency_efficiency_ratio</v>
+      </c>
+      <c r="I24" t="s">
+        <v>163</v>
+      </c>
+      <c r="J24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_total_latency_efficiency_ratio</v>
+      </c>
+      <c r="I25" t="s">
+        <v>164</v>
+      </c>
+      <c r="J25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_start_timestamp_seconds</v>
+      </c>
+      <c r="I26" t="s">
+        <v>165</v>
+      </c>
+      <c r="J26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_stop_timestamp_seconds</v>
+      </c>
+      <c r="I27" t="s">
+        <v>166</v>
+      </c>
+      <c r="J27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_duration_seconds</v>
+      </c>
+      <c r="I28" t="s">
+        <v>167</v>
+      </c>
+      <c r="J28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_count</v>
+      </c>
+      <c r="I29" t="s">
+        <v>168</v>
+      </c>
+      <c r="J29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_size_bytes_total</v>
+      </c>
+      <c r="I30" t="s">
+        <v>169</v>
+      </c>
+      <c r="J30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_average_size_bytes</v>
+      </c>
+      <c r="I31" t="s">
+        <v>169</v>
+      </c>
+      <c r="J31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_per_second_ratio</v>
+      </c>
+      <c r="I32" t="s">
+        <v>170</v>
+      </c>
+      <c r="J32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_data_errors_total</v>
+      </c>
+      <c r="I33" t="s">
+        <v>171</v>
+      </c>
+      <c r="J33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_data_error_rate_ratio</v>
+      </c>
+      <c r="I34" t="s">
+        <v>172</v>
+      </c>
+      <c r="J34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_record_success_rate_ratio</v>
+      </c>
+      <c r="I35" t="s">
+        <v>173</v>
+      </c>
+      <c r="J35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_start_timestamp_seconds</v>
+      </c>
+      <c r="I36" t="s">
+        <v>174</v>
+      </c>
+      <c r="J36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_stop_timestamp_seconds</v>
+      </c>
+      <c r="I37" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_duration_seconds</v>
+      </c>
+      <c r="I38" t="s">
+        <v>176</v>
+      </c>
+      <c r="J38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_count</v>
+      </c>
+      <c r="I39" t="s">
+        <v>177</v>
+      </c>
+      <c r="J39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="10"/>
+        <v>_</v>
+      </c>
+      <c r="E40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G40" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_average_size_bytes</v>
+      </c>
+      <c r="I40" t="s">
+        <v>177</v>
+      </c>
+      <c r="J40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" ref="D41:D47" si="11">IF(C41="","","_")</f>
+        <v>_</v>
+      </c>
+      <c r="E41" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G41" t="s">
+        <v>51</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_size_bytes_total</v>
+      </c>
+      <c r="I41" t="s">
+        <v>178</v>
+      </c>
+      <c r="J41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="11"/>
+        <v>_</v>
+      </c>
+      <c r="E42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_per_second_ratio</v>
+      </c>
+      <c r="I42" t="s">
+        <v>179</v>
+      </c>
+      <c r="J42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="11"/>
+        <v>_</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G43" t="s">
+        <v>35</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_io_bytes</v>
+      </c>
+      <c r="I43" t="s">
+        <v>142</v>
+      </c>
+      <c r="J43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="11"/>
+        <v>_</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G44" t="s">
+        <v>35</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_io_bytes</v>
+      </c>
+      <c r="I44" t="s">
+        <v>143</v>
+      </c>
+      <c r="J44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="11"/>
+        <v>_</v>
+      </c>
+      <c r="E45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G45" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_db_bytes</v>
+      </c>
+      <c r="I45" t="s">
+        <v>144</v>
+      </c>
+      <c r="J45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="11"/>
+        <v>_</v>
+      </c>
+      <c r="E46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_average_pct_ratio</v>
+      </c>
+      <c r="I46" t="s">
+        <v>145</v>
+      </c>
+      <c r="J46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="11"/>
+        <v>_</v>
+      </c>
+      <c r="E47" t="s">
+        <v>75</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="3"/>
+        <v>_</v>
+      </c>
+      <c r="G47" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>appstorestream_average_pct_ratio</v>
+      </c>
+      <c r="I47" t="s">
+        <v>146</v>
+      </c>
+      <c r="J47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2950531-C7B5-4438-9CD8-559C62D7D973}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -7310,7 +9075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5D793F-7895-4A1B-966E-2548BCE68562}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -7371,7 +9136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFB38DA-BF6E-4C1D-A544-185BFA3EE813}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>